<commit_message>
adding mode to only print models with instances
</commit_message>
<xml_diff>
--- a/examples/sbtab/template.xlsx
+++ b/examples/sbtab/template.xlsx
@@ -154,10 +154,10 @@
     <t>'!!rxnconReactionList'!A1</t>
   </si>
   <si>
-    <t>!!!ObjTables schema='SBtab' objTablesVersion='1.0.1' date='2020-07-07 21:43:42'</t>
-  </si>
-  <si>
-    <t>!!ObjTables schema='SBtab' type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!!ObjTables schema='SBtab' objTablesVersion='1.0.1' date='2020-07-07 22:05:32'</t>
+  </si>
+  <si>
+    <t>!!ObjTables schema='SBtab' type='TableOfContents' tableFormat='row' description='Table of contents' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Table</t>
@@ -253,7 +253,7 @@
     <t>rxnconReactionList</t>
   </si>
   <si>
-    <t>!!ObjTables type='Schema' tableFormat='row' name='SBtab' description='Table/model and column/attribute definitions' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables type='Schema' tableFormat='row' name='SBtab' description='Table/model and column/attribute definitions' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Name</t>
@@ -2116,7 +2116,7 @@
     <t>Reaction string</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Compartment' name='Compartment' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Compartment' name='Compartment' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Comment</t>
@@ -2170,7 +2170,7 @@
     <t>!Identifiers:sbo.go</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Compound' name='Compound' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Compound' name='Compound' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!SBML:species:id</t>
@@ -2233,7 +2233,7 @@
     <t>!NameForPlots</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Definition' name='Definition' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Definition' name='Definition' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!ComponentName</t>
@@ -2245,7 +2245,7 @@
     <t>!IsPartOf</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Enzyme' name='Enzyme' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Enzyme' name='Enzyme' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!CatalysedReaction</t>
@@ -2266,7 +2266,7 @@
     <t>!Gene</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='FbcObjective' name='FbcObjective' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='FbcObjective' name='FbcObjective' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!SBML:fbc:type</t>
@@ -2281,7 +2281,7 @@
     <t>!SBML:fbc:reaction</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Gene' name='Gene' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Gene' name='Gene' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!LocusName</t>
@@ -2311,7 +2311,7 @@
     <t>!SBML:fbc:Label</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Layout' name='Layout' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Layout' name='Layout' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!SBML:layout:modelEntity</t>
@@ -2347,7 +2347,7 @@
     <t>!SBML:layout:speciesRole</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Measurement' name='Measurement' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Measurement' name='Measurement' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Sample</t>
@@ -2359,7 +2359,7 @@
     <t>!ValueType</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='PbConfig' name='PbConfig' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='PbConfig' name='PbConfig' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Option</t>
@@ -2368,16 +2368,16 @@
     <t>!Value</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Position' name='Position' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Position' name='Position' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Element</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Protein' name='Protein' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
-  </si>
-  <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Quantity' name='Quantity' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Protein' name='Protein' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
+  </si>
+  <si>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Quantity' name='Quantity' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Quantity</t>
@@ -2539,7 +2539,7 @@
     <t>!Parameter:SBML:parameter:id</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='QuantityInfo' name='QuantityInfo' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='QuantityInfo' name='QuantityInfo' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Constant</t>
@@ -2557,7 +2557,7 @@
     <t>!SBMLElementType</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='QuantityMatrix' name='QuantityMatrix' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='QuantityMatrix' name='QuantityMatrix' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!&gt;Table:Column</t>
@@ -2596,7 +2596,7 @@
     <t>!&gt;TP:t1:std</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Reaction' name='Reaction' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Reaction' name='Reaction' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Modifier</t>
@@ -2668,7 +2668,7 @@
     <t>!Regulator</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='ReactionStoichiometry' name='ReactionStoichiometry' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='ReactionStoichiometry' name='ReactionStoichiometry' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Stoichiometry</t>
@@ -2680,7 +2680,7 @@
     <t>!Product</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Regulator' name='Regulator' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Regulator' name='Regulator' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!TargetGene</t>
@@ -2692,7 +2692,7 @@
     <t>!TargetPromoter</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Relation' name='Relation' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Relation' name='Relation' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!FromObject</t>
@@ -2707,13 +2707,13 @@
     <t>!Value:QuantityType</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Relationship' name='Relationship' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='Relationship' name='Relationship' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!Relation</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrix' name='SparseMatrix' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrix' name='SparseMatrix' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!RowID</t>
@@ -2722,13 +2722,13 @@
     <t>!ColumnID</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixColumn' name='SparseMatrixColumn' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixColumn' name='SparseMatrixColumn' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!ColumnString</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixOrdered' name='SparseMatrixOrdered' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixOrdered' name='SparseMatrixOrdered' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!RowNumber</t>
@@ -2737,19 +2737,19 @@
     <t>!ColumnNumber</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixRow' name='SparseMatrixRow' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='SparseMatrixRow' name='SparseMatrixRow' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!RowString</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='StoichiometricMatrix' name='StoichiometricMatrix' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='StoichiometricMatrix' name='StoichiometricMatrix' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!ReactionID</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='rxnconContingencyList' name='rxnconContingencyList' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='rxnconContingencyList' name='rxnconContingencyList' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!UID:Contingency</t>
@@ -2770,7 +2770,7 @@
     <t>!InternalComplexID</t>
   </si>
   <si>
-    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='rxnconReactionList' name='rxnconReactionList' date='2020-07-07 21:43:42' objTablesVersion='1.0.1'</t>
+    <t>!!ObjTables schema='SBtab' type='Data' tableFormat='row' class='rxnconReactionList' name='rxnconReactionList' date='2020-07-07 22:05:32' objTablesVersion='1.0.1'</t>
   </si>
   <si>
     <t>!UID:Reaction</t>

</xml_diff>